<commit_message>
f y h excel
</commit_message>
<xml_diff>
--- a/t2 - copia.xlsx
+++ b/t2 - copia.xlsx
@@ -5,17 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franr\Desktop\Universidad\7mo semestre\Logaritmos\t2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franr\Desktop\Universidad\7mo semestre\Logaritmos\t2\t2log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C32CD30-2F15-4288-B648-0720193955EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683C3C1E-8A62-48B7-906E-57A04D422BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2^10" sheetId="4" r:id="rId1"/>
-    <sheet name="2^12" sheetId="3" r:id="rId2"/>
-    <sheet name="2^14" sheetId="1" r:id="rId3"/>
+    <sheet name="Fibonacci 2^10" sheetId="8" r:id="rId1"/>
+    <sheet name="Fibonacci 2^12" sheetId="7" r:id="rId2"/>
+    <sheet name="Fibonacci 2^14" sheetId="6" r:id="rId3"/>
+    <sheet name="Heap 2^10" sheetId="4" r:id="rId4"/>
+    <sheet name="Heap 2^12" sheetId="3" r:id="rId5"/>
+    <sheet name="Heap 2^14" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="1">
   <si>
     <t>Aristas</t>
   </si>
@@ -366,7 +369,208 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9E4593-669B-4C0E-9E28-E9F234AC4382}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A8" si="0">A3+1</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A605B0F-27B5-4D2E-93D6-20E3AB4CF8D4}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A8" si="0">A3+1</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF17DE8-4563-4441-BEDE-F2AD606576A5}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A8" si="0">A3+1</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7993EC9-C3C3-4B23-99FD-33A21524D442}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -426,12 +630,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A61D9CF-2909-413A-BF24-52051564F9B5}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,12 +694,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>